<commit_message>
update accession loader to use vavilov accession format files
</commit_message>
<xml_diff>
--- a/vavilov_pedigree/test/data/accessions.xlsx
+++ b/vavilov_pedigree/test/data/accessions.xlsx
@@ -22,10 +22,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
-    <t xml:space="preserve">Accession</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CollectingNumber</t>
+    <t xml:space="preserve">CODE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COLLECTING CODE</t>
   </si>
   <si>
     <t xml:space="preserve">acc1</t>
@@ -173,13 +173,10 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">

</xml_diff>